<commit_message>
Update: facturacion en proceso
</commit_message>
<xml_diff>
--- a/core/Report/ticket.xlsx
+++ b/core/Report/ticket.xlsx
@@ -11,24 +11,115 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="57" uniqueCount="30">
   <si>
     <t>Id</t>
   </si>
   <si>
-    <t>identificacion</t>
-  </si>
-  <si>
-    <t>razon_social</t>
-  </si>
-  <si>
-    <t>total</t>
-  </si>
-  <si>
-    <t>9999999999001</t>
-  </si>
-  <si>
-    <t>PRUEBAS SERVICIO DE RENTAS INTERNAS</t>
+    <t>Codigo</t>
+  </si>
+  <si>
+    <t>Operador</t>
+  </si>
+  <si>
+    <t>saldo</t>
+  </si>
+  <si>
+    <t>Desde</t>
+  </si>
+  <si>
+    <t>Hasta</t>
+  </si>
+  <si>
+    <t>Comentario</t>
+  </si>
+  <si>
+    <t>admin_1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2022/12/07
+02:16:57</t>
+  </si>
+  <si>
+    <t>Pendiente</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023/01/07
+02:33:33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023/01/07
+02:37:17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023/01/07
+02:43:14</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023/01/07
+02:47:41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023/01/07
+14:00:00</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023/01/07
+17:00:00</t>
+  </si>
+  <si>
+    <t>Finalizado\</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023/01/09
+18:23:47</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023/01/09
+18:29:23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023/01/09
+18:36:05</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023/01/09
+18:40:37</t>
+  </si>
+  <si>
+    <t>Finalizado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023/01/09
+18:40:46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023/01/09
+18:41:04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023/01/09
+18:43:50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023/01/09
+18:49:04</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023/01/09
+22:37:24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023/01/09
+22:37:34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023/01/09
+22:37:38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">2023/01/09
+22:38:02</t>
   </si>
 </sst>
 </file>
@@ -405,16 +496,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:G16"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <cols>
     <col min="1" max="1" width="4" customWidth="1"/>
-    <col min="2" max="2" width="16" customWidth="1"/>
-    <col min="3" max="3" width="14" customWidth="1"/>
-    <col min="4" max="4" width="7" customWidth="1"/>
+    <col min="2" max="2" width="8" customWidth="1"/>
+    <col min="3" max="3" width="10" customWidth="1"/>
+    <col min="4" max="6" width="7" customWidth="1"/>
+    <col min="7" max="7" width="12" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -427,47 +519,329 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
+      <c r="B2">
+        <v>75</v>
       </c>
       <c r="C2" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>300</v>
+      </c>
+      <c r="E2" t="s">
+        <v>8</v>
+      </c>
+      <c r="G2" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>2</v>
       </c>
-      <c r="B3" t="s">
-        <v>4</v>
+      <c r="B3">
+        <v>76</v>
       </c>
       <c r="C3" t="s">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="D3">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>0</v>
+      </c>
+      <c r="E3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G3" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
+      <c r="B4">
+        <v>77</v>
+      </c>
+      <c r="C4" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4">
+        <v>0</v>
+      </c>
+      <c r="E4" t="s">
+        <v>11</v>
+      </c>
+      <c r="G4" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5">
         <v>4</v>
       </c>
-      <c r="C4" t="s">
+      <c r="B5">
+        <v>78</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
+      </c>
+      <c r="D5">
+        <v>0</v>
+      </c>
+      <c r="E5" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6">
         <v>5</v>
       </c>
-      <c r="D4">
-        <v>3</v>
+      <c r="B6">
+        <v>79</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6">
+        <v>0</v>
+      </c>
+      <c r="E6" t="s">
+        <v>13</v>
+      </c>
+      <c r="G6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7">
+        <v>73</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7">
+        <v>0</v>
+      </c>
+      <c r="E7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" t="s">
+        <v>15</v>
+      </c>
+      <c r="G7" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8">
+        <v>74</v>
+      </c>
+      <c r="C8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D8">
+        <v>20</v>
+      </c>
+      <c r="E8" t="s">
+        <v>14</v>
+      </c>
+      <c r="G8" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9">
+        <v>80</v>
+      </c>
+      <c r="C9" t="s">
+        <v>7</v>
+      </c>
+      <c r="D9">
+        <v>0</v>
+      </c>
+      <c r="E9" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10">
+        <v>81</v>
+      </c>
+      <c r="C10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D10">
+        <v>0</v>
+      </c>
+      <c r="E10" t="s">
+        <v>18</v>
+      </c>
+      <c r="G10" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11">
+        <v>82</v>
+      </c>
+      <c r="C11" t="s">
+        <v>7</v>
+      </c>
+      <c r="D11">
+        <v>0</v>
+      </c>
+      <c r="E11" t="s">
+        <v>19</v>
+      </c>
+      <c r="F11" t="s">
+        <v>20</v>
+      </c>
+      <c r="G11" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12">
+        <v>83</v>
+      </c>
+      <c r="C12" t="s">
+        <v>7</v>
+      </c>
+      <c r="D12">
+        <v>0</v>
+      </c>
+      <c r="E12" t="s">
+        <v>22</v>
+      </c>
+      <c r="F12" t="s">
+        <v>23</v>
+      </c>
+      <c r="G12" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13">
+        <v>84</v>
+      </c>
+      <c r="C13" t="s">
+        <v>7</v>
+      </c>
+      <c r="D13">
+        <v>0</v>
+      </c>
+      <c r="E13" t="s">
+        <v>24</v>
+      </c>
+      <c r="G13" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14">
+        <v>85</v>
+      </c>
+      <c r="C14" t="s">
+        <v>7</v>
+      </c>
+      <c r="D14">
+        <v>0</v>
+      </c>
+      <c r="E14" t="s">
+        <v>25</v>
+      </c>
+      <c r="F14" t="s">
+        <v>26</v>
+      </c>
+      <c r="G14" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15">
+        <v>86</v>
+      </c>
+      <c r="C15" t="s">
+        <v>7</v>
+      </c>
+      <c r="D15">
+        <v>0</v>
+      </c>
+      <c r="E15" t="s">
+        <v>27</v>
+      </c>
+      <c r="F15" t="s">
+        <v>28</v>
+      </c>
+      <c r="G15" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16">
+        <v>87</v>
+      </c>
+      <c r="C16" t="s">
+        <v>7</v>
+      </c>
+      <c r="D16">
+        <v>0</v>
+      </c>
+      <c r="E16" t="s">
+        <v>29</v>
+      </c>
+      <c r="G16" t="s">
+        <v>9</v>
       </c>
     </row>
   </sheetData>

</xml_diff>